<commit_message>
Updated Bela mini BOM to fix missing resistors and socket
</commit_message>
<xml_diff>
--- a/pocketbela-cape/belamini_cape_rev_B1/PocketBelaCape_rev2_bom.xlsx
+++ b/pocketbela-cape/belamini_cape_rev_B1/PocketBelaCape_rev2_bom.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="102">
   <si>
     <t>Name</t>
   </si>
@@ -221,13 +221,13 @@
     <t>J2</t>
   </si>
   <si>
-    <t>DNI</t>
-  </si>
-  <si>
     <t>3-pin header</t>
   </si>
   <si>
-    <t>-</t>
+    <t>3-pin socket</t>
+  </si>
+  <si>
+    <t>855-M20-7820346</t>
   </si>
   <si>
     <t>J3, J4</t>
@@ -284,6 +284,12 @@
     <t>100 ohm</t>
   </si>
   <si>
+    <t>R4, R5</t>
+  </si>
+  <si>
+    <t>560 ohm</t>
+  </si>
+  <si>
     <t>RN1</t>
   </si>
   <si>
@@ -311,7 +317,7 @@
     <t>Total</t>
   </si>
   <si>
-    <t>BOM rev. A1</t>
+    <t>BOM rev. B1</t>
   </si>
 </sst>
 </file>
@@ -1578,7 +1584,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2057,23 +2063,25 @@
       <c r="A16" t="s" s="7">
         <v>68</v>
       </c>
-      <c r="B16" t="s" s="6">
+      <c r="B16" s="8">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s" s="6">
         <v>69</v>
       </c>
-      <c r="C16" t="s" s="6">
-        <v>70</v>
-      </c>
       <c r="D16" t="s" s="6">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="E16" t="s" s="6">
         <v>66</v>
       </c>
       <c r="F16" t="s" s="6">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G16" s="5"/>
-      <c r="H16" s="6"/>
+      <c r="H16" t="s" s="6">
+        <v>71</v>
+      </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
@@ -2234,7 +2242,7 @@
         <v>90</v>
       </c>
       <c r="B22" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" t="s" s="6">
         <v>91</v>
@@ -2246,11 +2254,9 @@
         <v>13</v>
       </c>
       <c r="F22" t="s" s="6">
-        <v>92</v>
-      </c>
-      <c r="G22" s="8">
-        <v>2060086</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
@@ -2259,29 +2265,29 @@
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
     </row>
-    <row r="23" ht="26.7" customHeight="1">
+    <row r="23" ht="15" customHeight="1">
       <c r="A23" t="s" s="7">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B23" s="8">
         <v>1</v>
       </c>
-      <c r="C23" t="s" s="10">
+      <c r="C23" t="s" s="6">
+        <v>93</v>
+      </c>
+      <c r="D23" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s" s="6">
+        <v>13</v>
+      </c>
+      <c r="F23" t="s" s="6">
         <v>94</v>
       </c>
-      <c r="D23" t="s" s="6">
-        <v>36</v>
-      </c>
-      <c r="E23" t="s" s="6">
-        <v>95</v>
-      </c>
-      <c r="F23" t="s" s="6">
-        <v>96</v>
-      </c>
-      <c r="G23" s="9"/>
-      <c r="H23" t="s" s="6">
-        <v>97</v>
-      </c>
+      <c r="G23" s="8">
+        <v>2060086</v>
+      </c>
+      <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
@@ -2289,15 +2295,29 @@
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
     </row>
-    <row r="24" ht="14.7" customHeight="1">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
+    <row r="24" ht="26.7" customHeight="1">
+      <c r="A24" t="s" s="7">
+        <v>95</v>
+      </c>
+      <c r="B24" s="8">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s" s="10">
+        <v>96</v>
+      </c>
+      <c r="D24" t="s" s="6">
+        <v>36</v>
+      </c>
+      <c r="E24" t="s" s="6">
+        <v>97</v>
+      </c>
+      <c r="F24" t="s" s="6">
+        <v>98</v>
+      </c>
+      <c r="G24" s="9"/>
+      <c r="H24" t="s" s="6">
+        <v>99</v>
+      </c>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
@@ -2305,18 +2325,13 @@
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
     </row>
-    <row r="25" ht="15" customHeight="1">
-      <c r="A25" t="s" s="7">
-        <v>98</v>
-      </c>
-      <c r="B25" s="8">
-        <f>SUM(B3:B23)</f>
-        <v>44</v>
-      </c>
+    <row r="25" ht="14.7" customHeight="1">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
       <c r="C25" s="5"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="6"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
@@ -2326,13 +2341,18 @@
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
     </row>
-    <row r="26" ht="14.7" customHeight="1">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
+    <row r="26" ht="15" customHeight="1">
+      <c r="A26" t="s" s="7">
+        <v>100</v>
+      </c>
+      <c r="B26" s="8">
+        <f>SUM(B3:B24)</f>
+        <v>47</v>
+      </c>
       <c r="C26" s="5"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="5"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="6"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
@@ -2346,8 +2366,8 @@
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
@@ -2359,10 +2379,8 @@
       <c r="N27" s="5"/>
     </row>
     <row r="28" ht="14.7" customHeight="1">
-      <c r="A28" t="s" s="7">
-        <v>99</v>
-      </c>
-      <c r="B28" s="11"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
@@ -2377,8 +2395,10 @@
       <c r="N28" s="5"/>
     </row>
     <row r="29" ht="14.7" customHeight="1">
-      <c r="A29" s="4"/>
-      <c r="B29" s="5"/>
+      <c r="A29" t="s" s="7">
+        <v>101</v>
+      </c>
+      <c r="B29" s="11"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
@@ -2488,6 +2508,22 @@
       <c r="M35" s="5"/>
       <c r="N35" s="5"/>
     </row>
+    <row r="36" ht="14.7" customHeight="1">
+      <c r="A36" s="4"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>

</xml_diff>